<commit_message>
fixed URIs for CPV version 0.7 and CPV-aligns ontologies. Changed code for person-tilte controlled vocabulary in order to have homogeneous URIs in English for all the vocabulary items;revision of metadata of person-title controlled vocabulary
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-people/person-title/person-title.xlsx
+++ b/VocabolariControllati/classifications-for-people/person-title/person-title.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lgu/Dropbox/repository/workspace_oxy/daf-ontologie-vocabolari-controllati/VocabolariControllati/classifications-for-people/person-title/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Desktop/AGID/NuovoDATIGOV/DAF/Git/OntologieVocabolariControllati/VocabolariControllati/classifications-for-people/person-title/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27D0B16D-F168-2B49-AED5-90EAEC4B016F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A65C9EA-407F-F84D-BF75-18CF4F403D94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14460" xr2:uid="{B3AEB04A-E60E-AF49-9A69-067D47AA27AD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Mrs</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Abbreviazione di 'Dottoressa'.</t>
   </si>
   <si>
-    <t>Dott.sa</t>
-  </si>
-  <si>
     <t>codice_1_livello</t>
   </si>
   <si>
@@ -103,6 +100,21 @@
   </si>
   <si>
     <t>definizione_ENG</t>
+  </si>
+  <si>
+    <t>Prof.ssa</t>
+  </si>
+  <si>
+    <t>Ms</t>
+  </si>
+  <si>
+    <t>English honorific used with the last name or full name of a woman, intended as a default form of address for women regardless of marital status</t>
+  </si>
+  <si>
+    <t>Dott.ssa</t>
+  </si>
+  <si>
+    <t>Abbreviazione di 'Professoressa'</t>
   </si>
 </sst>
 </file>
@@ -454,37 +466,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A37C2D4-51ED-D440-9B4E-4271C6A5FD5B}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="194" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -500,59 +514,53 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -568,14 +576,42 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>20</v>
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>